<commit_message>
grafico de correlação linear e regressão linear
</commit_message>
<xml_diff>
--- a/database/case_analista_de_bi_pleno.xlsx
+++ b/database/case_analista_de_bi_pleno.xlsx
@@ -109,13 +109,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="10" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,10 +733,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M18"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O15" sqref="O15"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -825,7 +826,7 @@
         <v>5.8400000000000001E-2</v>
       </c>
       <c r="J2" s="2">
-        <v>8.4900000000000003E-2</v>
+        <v>8.2100000000000006E-2</v>
       </c>
       <c r="K2">
         <v>195099122</v>
@@ -866,7 +867,7 @@
         <v>5.91E-2</v>
       </c>
       <c r="J3" s="2">
-        <v>8.2100000000000006E-2</v>
+        <v>0.1091</v>
       </c>
       <c r="K3">
         <v>197061065</v>
@@ -907,7 +908,7 @@
         <v>6.4100000000000004E-2</v>
       </c>
       <c r="J4" s="2">
-        <v>0.1091</v>
+        <v>0.13289999999999999</v>
       </c>
       <c r="K4">
         <v>198836089</v>
@@ -948,7 +949,7 @@
         <v>0.1067</v>
       </c>
       <c r="J5" s="2">
-        <v>0.13289999999999999</v>
+        <v>0.14019999999999999</v>
       </c>
       <c r="K5">
         <v>200401258</v>
@@ -989,7 +990,7 @@
         <v>6.2899999999999998E-2</v>
       </c>
       <c r="J6" s="2">
-        <v>0.14019999999999999</v>
+        <v>9.9699999999999997E-2</v>
       </c>
       <c r="K6">
         <v>201728051</v>
@@ -1030,7 +1031,7 @@
         <v>2.9499999999999998E-2</v>
       </c>
       <c r="J7" s="2">
-        <v>9.9699999999999997E-2</v>
+        <v>6.4199999999999993E-2</v>
       </c>
       <c r="K7">
         <v>202790459</v>
@@ -1071,7 +1072,7 @@
         <v>3.7499999999999999E-2</v>
       </c>
       <c r="J8" s="2">
-        <v>6.4199999999999993E-2</v>
+        <v>5.9400000000000001E-2</v>
       </c>
       <c r="K8">
         <v>203554092</v>
@@ -1112,7 +1113,7 @@
         <v>4.3099999999999999E-2</v>
       </c>
       <c r="J9" s="2">
-        <v>5.9400000000000001E-2</v>
+        <v>2.75E-2</v>
       </c>
       <c r="K9">
         <v>203993710</v>
@@ -1153,7 +1154,7 @@
         <v>4.5199999999999997E-2</v>
       </c>
       <c r="J10" s="2">
-        <v>2.75E-2</v>
+        <v>4.4600000000000001E-2</v>
       </c>
       <c r="K10">
         <v>204080793</v>
@@ -1194,7 +1195,7 @@
         <v>0.10059999999999999</v>
       </c>
       <c r="J11" s="2">
-        <v>4.4600000000000001E-2</v>
+        <v>0.1239</v>
       </c>
       <c r="K11">
         <v>203785465</v>
@@ -1235,7 +1236,7 @@
         <v>5.79E-2</v>
       </c>
       <c r="J12" s="2">
-        <v>0.1239</v>
+        <v>0.1305</v>
       </c>
       <c r="K12">
         <v>203080756</v>
@@ -1276,7 +1277,7 @@
         <v>4.6199999999999998E-2</v>
       </c>
       <c r="J13" s="2">
-        <v>0.1305</v>
+        <v>0.1089</v>
       </c>
       <c r="K13">
         <v>203997347</v>
@@ -1317,7 +1318,7 @@
         <v>4.8300000000000003E-2</v>
       </c>
       <c r="J14" s="2">
-        <v>0.1089</v>
+        <v>0.15</v>
       </c>
       <c r="K14">
         <v>204861525</v>
@@ -1328,6 +1329,9 @@
       <c r="M14">
         <v>6000000</v>
       </c>
+    </row>
+    <row r="18" spans="9:9" x14ac:dyDescent="0.25">
+      <c r="I18" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>